<commit_message>
Add some results of GA and implement tabu search.
</commit_message>
<xml_diff>
--- a/data/RESULTS.xlsx
+++ b/data/RESULTS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -416,8 +416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,11 +458,17 @@
       <c r="C2" s="1">
         <v>9555</v>
       </c>
+      <c r="D2">
+        <v>596</v>
+      </c>
       <c r="F2" s="1">
         <v>78658</v>
       </c>
       <c r="G2" s="1">
         <v>9555</v>
+      </c>
+      <c r="H2" s="1">
+        <v>596</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -475,11 +481,17 @@
       <c r="C3">
         <v>9556</v>
       </c>
-      <c r="F3">
+      <c r="D3">
+        <v>596</v>
+      </c>
+      <c r="F3" s="2">
         <v>78659</v>
       </c>
       <c r="G3">
         <v>9556</v>
+      </c>
+      <c r="H3">
+        <v>597</v>
       </c>
       <c r="J3">
         <v>85214</v>
@@ -498,11 +510,17 @@
       <c r="C4">
         <v>9582</v>
       </c>
-      <c r="F4">
+      <c r="D4" s="2">
+        <v>593</v>
+      </c>
+      <c r="F4" s="2">
         <v>78659</v>
       </c>
       <c r="G4" s="3">
         <v>9730</v>
+      </c>
+      <c r="H4" s="3">
+        <v>597</v>
       </c>
       <c r="J4">
         <v>78662</v>
@@ -521,11 +539,17 @@
       <c r="C5">
         <v>9609</v>
       </c>
+      <c r="D5">
+        <v>597</v>
+      </c>
       <c r="F5" s="3">
         <v>78660</v>
       </c>
       <c r="G5" s="3">
         <v>9557</v>
+      </c>
+      <c r="H5" s="3">
+        <v>597</v>
       </c>
       <c r="J5" s="3">
         <v>78661</v>
@@ -544,11 +568,17 @@
       <c r="C6">
         <v>9608</v>
       </c>
+      <c r="D6">
+        <v>597</v>
+      </c>
       <c r="F6" s="3">
         <v>78660</v>
       </c>
       <c r="G6" s="3">
         <v>9613</v>
+      </c>
+      <c r="H6" s="3">
+        <v>603</v>
       </c>
       <c r="J6" s="3">
         <v>78661</v>
@@ -567,11 +597,17 @@
       <c r="C7">
         <v>9553</v>
       </c>
+      <c r="D7">
+        <v>597</v>
+      </c>
       <c r="F7" s="3">
         <v>78660</v>
       </c>
       <c r="G7" s="3">
         <v>9556</v>
+      </c>
+      <c r="H7" s="3">
+        <v>596</v>
       </c>
       <c r="J7">
         <v>78660</v>
@@ -590,11 +626,17 @@
       <c r="C8">
         <v>9556</v>
       </c>
+      <c r="D8">
+        <v>597</v>
+      </c>
       <c r="F8" s="3">
         <v>78660</v>
       </c>
       <c r="G8" s="3">
         <v>9556</v>
+      </c>
+      <c r="H8" s="3">
+        <v>596</v>
       </c>
       <c r="J8">
         <v>78662</v>
@@ -613,11 +655,17 @@
       <c r="C9">
         <v>9556</v>
       </c>
+      <c r="D9">
+        <v>597</v>
+      </c>
       <c r="F9" s="3">
         <v>78671</v>
       </c>
       <c r="G9" s="3">
         <v>9555</v>
+      </c>
+      <c r="H9" s="3">
+        <v>597</v>
       </c>
       <c r="J9">
         <v>78660</v>
@@ -636,11 +684,17 @@
       <c r="C10">
         <v>9554</v>
       </c>
+      <c r="D10" s="2">
+        <v>593</v>
+      </c>
       <c r="F10" s="3">
         <v>78685</v>
       </c>
       <c r="G10" s="3">
         <v>9556</v>
+      </c>
+      <c r="H10" s="3">
+        <v>597</v>
       </c>
       <c r="J10">
         <v>78660</v>
@@ -659,11 +713,17 @@
       <c r="C11" s="2">
         <v>9553</v>
       </c>
+      <c r="D11">
+        <v>597</v>
+      </c>
       <c r="F11" s="3">
         <v>78660</v>
       </c>
       <c r="G11" s="3">
         <v>9560</v>
+      </c>
+      <c r="H11" s="3">
+        <v>597</v>
       </c>
       <c r="J11">
         <v>85029</v>
@@ -682,11 +742,17 @@
       <c r="C12" s="2">
         <v>9553</v>
       </c>
+      <c r="D12">
+        <v>597</v>
+      </c>
       <c r="F12" s="3">
         <v>78660</v>
       </c>
       <c r="G12" s="3">
         <v>9612</v>
+      </c>
+      <c r="H12" s="3">
+        <v>597</v>
       </c>
       <c r="J12">
         <v>78662</v>
@@ -705,11 +771,17 @@
       <c r="C13">
         <v>9613</v>
       </c>
+      <c r="D13">
+        <v>596</v>
+      </c>
       <c r="F13" s="3">
         <v>78664</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="2">
         <v>9553</v>
+      </c>
+      <c r="H13" s="2">
+        <v>593</v>
       </c>
       <c r="J13" s="2">
         <v>78660</v>
@@ -728,11 +800,17 @@
       <c r="C14">
         <v>9621</v>
       </c>
+      <c r="D14" s="2">
+        <v>593</v>
+      </c>
       <c r="F14" s="3">
         <v>78667</v>
       </c>
       <c r="G14" s="3">
         <v>9559</v>
+      </c>
+      <c r="H14" s="2">
+        <v>593</v>
       </c>
       <c r="J14">
         <v>78661</v>
@@ -751,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,11 +871,17 @@
       <c r="C2" s="1">
         <v>9555</v>
       </c>
+      <c r="D2" s="1">
+        <v>596</v>
+      </c>
       <c r="F2" s="1">
         <v>78658</v>
       </c>
       <c r="G2" s="1">
         <v>9555</v>
+      </c>
+      <c r="H2" s="1">
+        <v>596</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -810,8 +894,17 @@
       <c r="C3">
         <v>9566</v>
       </c>
+      <c r="D3">
+        <v>597</v>
+      </c>
+      <c r="F3">
+        <v>78741</v>
+      </c>
       <c r="G3">
         <v>9559</v>
+      </c>
+      <c r="H3">
+        <v>596</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -824,8 +917,17 @@
       <c r="C4">
         <v>9567</v>
       </c>
+      <c r="D4">
+        <v>597</v>
+      </c>
+      <c r="F4">
+        <v>78664</v>
+      </c>
       <c r="G4">
         <v>9554</v>
+      </c>
+      <c r="H4">
+        <v>596</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -838,8 +940,17 @@
       <c r="C5">
         <v>9663</v>
       </c>
-      <c r="G5">
+      <c r="D5">
+        <v>598</v>
+      </c>
+      <c r="F5">
+        <v>78661</v>
+      </c>
+      <c r="G5" s="2">
         <v>9551</v>
+      </c>
+      <c r="H5">
+        <v>596</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -852,8 +963,17 @@
       <c r="C6">
         <v>9557</v>
       </c>
+      <c r="D6">
+        <v>596</v>
+      </c>
+      <c r="F6">
+        <v>78665</v>
+      </c>
       <c r="G6">
         <v>9557</v>
+      </c>
+      <c r="H6">
+        <v>596</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -866,8 +986,17 @@
       <c r="C7">
         <v>9557</v>
       </c>
+      <c r="D7">
+        <v>596</v>
+      </c>
+      <c r="F7">
+        <v>78661</v>
+      </c>
       <c r="G7">
         <v>9557</v>
+      </c>
+      <c r="H7">
+        <v>597</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -880,8 +1009,17 @@
       <c r="C8">
         <v>9576</v>
       </c>
+      <c r="D8">
+        <v>597</v>
+      </c>
+      <c r="F8">
+        <v>78663</v>
+      </c>
       <c r="G8">
         <v>9559</v>
+      </c>
+      <c r="H8">
+        <v>596</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -894,6 +1032,18 @@
       <c r="C9">
         <v>9553</v>
       </c>
+      <c r="D9">
+        <v>597</v>
+      </c>
+      <c r="F9">
+        <v>78700</v>
+      </c>
+      <c r="G9">
+        <v>9557</v>
+      </c>
+      <c r="H9">
+        <v>596</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -905,6 +1055,18 @@
       <c r="C10">
         <v>9556</v>
       </c>
+      <c r="D10">
+        <v>596</v>
+      </c>
+      <c r="F10">
+        <v>80053</v>
+      </c>
+      <c r="G10">
+        <v>9558</v>
+      </c>
+      <c r="H10">
+        <v>596</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -916,6 +1078,18 @@
       <c r="C11" s="2">
         <v>9552</v>
       </c>
+      <c r="D11">
+        <v>596</v>
+      </c>
+      <c r="F11">
+        <v>78662</v>
+      </c>
+      <c r="G11">
+        <v>9553</v>
+      </c>
+      <c r="H11">
+        <v>596</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -927,6 +1101,18 @@
       <c r="C12">
         <v>9554</v>
       </c>
+      <c r="D12">
+        <v>596</v>
+      </c>
+      <c r="F12">
+        <v>78663</v>
+      </c>
+      <c r="G12">
+        <v>9557</v>
+      </c>
+      <c r="H12">
+        <v>596</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -938,6 +1124,18 @@
       <c r="C13">
         <v>9558</v>
       </c>
+      <c r="D13">
+        <v>596</v>
+      </c>
+      <c r="F13">
+        <v>78663</v>
+      </c>
+      <c r="G13">
+        <v>9553</v>
+      </c>
+      <c r="H13">
+        <v>596</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -948,6 +1146,18 @@
       </c>
       <c r="C14">
         <v>9555</v>
+      </c>
+      <c r="D14">
+        <v>596</v>
+      </c>
+      <c r="F14">
+        <v>78662</v>
+      </c>
+      <c r="G14">
+        <v>9557</v>
+      </c>
+      <c r="H14">
+        <v>597</v>
       </c>
     </row>
   </sheetData>

</xml_diff>